<commit_message>
Data Driven for Add Batch MOdule pushed
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Testdata.xlsx
+++ b/src/test/resources/testData/Testdata.xlsx
@@ -5,17 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karthikaramesh/Documents/Numpy Ninja/LMS Hackathon/Submission doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karthikaramesh/eclipse-workspace/Team06_LMSPhase2_SeleniumHackers/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9957E923-C833-6146-B487-AD7FF8DF39A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1637F133-EE59-594C-9397-A5FEB8F4E63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{F6E5D68C-7B8C-0642-9B7E-6B6C909A101B}"/>
+    <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" xr2:uid="{E2C16CBD-B1C9-DE47-975A-34B2B7E9936C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Program" sheetId="1" r:id="rId1"/>
-    <sheet name="Batch" sheetId="2" r:id="rId2"/>
-    <sheet name="Class" sheetId="3" r:id="rId3"/>
+    <sheet name="Batch" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Class</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Program Name</t>
   </si>
@@ -53,13 +48,31 @@
   </si>
   <si>
     <t>Number of Classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> data driven 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> data driven 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> data driven 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> data driven 4</t>
+  </si>
+  <si>
+    <t>ChatBotTestuk</t>
+  </si>
+  <si>
+    <t>Splunk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +85,12 @@
       <sz val="16"/>
       <color rgb="FF495057"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -95,9 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,66 +451,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9495F50F-0AD3-534C-BBFA-5937C20D8514}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B5D65F-79F2-9E47-B153-49CB52F147B6}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735F5236-1767-0446-8018-7E26CAB96755}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.5" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="28.5" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="43.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513B0DE0-FE55-CE45-B46F-738A5542CBF2}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
integration between batch and class
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Testdata.xlsx
+++ b/src/test/resources/testData/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karthikaramesh/eclipse-workspace/Team06_LMSPhase2_SeleniumHackers/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5AF813-84AC-5443-AFDC-69BC8CB13476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB07385D-321A-CD44-AEBC-BF553CD2DEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" xr2:uid="{E2C16CBD-B1C9-DE47-975A-34B2B7E9936C}"/>
   </bookViews>
@@ -466,7 +466,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>9087</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Merged login and batch
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Testdata.xlsx
+++ b/src/test/resources/testData/Testdata.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karthikaramesh/eclipse-workspace/Team06_LMSPhase2_SeleniumHackers/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129CAC22-D9DB-634C-BC01-1433F439EB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839E9DBB-0A63-8946-BE79-62C853B49424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3480" yWindow="2560" windowWidth="27640" windowHeight="16940" xr2:uid="{E2C16CBD-B1C9-DE47-975A-34B2B7E9936C}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Program" sheetId="3" r:id="rId3"/>
+    <sheet name="Class" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Program Name</t>
   </si>
@@ -53,20 +56,53 @@
     <t>DD 1</t>
   </si>
   <si>
-    <t>EDGE</t>
-  </si>
-  <si>
-    <t>DD 2</t>
-  </si>
-  <si>
-    <t>DD 3</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Sdet@gmail.com</t>
+  </si>
+  <si>
+    <t>LmsHackathon@2024</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>5hcjask**(nnnn</t>
+  </si>
+  <si>
+    <t>&amp;^bjbjb@BJ</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>LMS - Learning Management System</t>
+  </si>
+  <si>
+    <t>LMS</t>
+  </si>
+  <si>
+    <t>Playwrite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +123,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF495057"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,14 +162,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735F5236-1767-0446-8018-7E26CAB96755}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,12 +535,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
+    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>222</v>
+        <v>789</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -487,42 +549,145 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>223</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>224</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54D2CBD6-3AEE-1648-BC08-08D118A5B666}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" tooltip="mailto:Sdet@gmail.com" xr:uid="{17779485-2D92-DF4B-AF71-885556CCFD29}"/>
+    <hyperlink ref="B2" r:id="rId2" tooltip="mailto:LmsHackathon@2024" xr:uid="{C2A308ED-9E76-F541-99C3-10461994CED6}"/>
+    <hyperlink ref="A4" r:id="rId3" tooltip="mailto:Sdet@gmail.com" xr:uid="{897E0B82-8330-A34B-ACB4-ED49D71A832A}"/>
+    <hyperlink ref="B5" r:id="rId4" tooltip="mailto:LmsHackathon@2024" xr:uid="{5D2A466B-D09A-6B42-A948-44086D20601A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81690B68-752F-1545-ADAC-8F651F2D421E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75742CB7-6785-3440-AF38-98A56A9BB621}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update for program delete validation
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Testdata.xlsx
+++ b/src/test/resources/testData/Testdata.xlsx
@@ -76,22 +76,22 @@
     <t>Name</t>
   </si>
   <si>
-    <t>OOPS</t>
+    <t>Azure</t>
   </si>
   <si>
-    <t>JavaOOPS</t>
+    <t>cloud</t>
   </si>
   <si>
-    <t>Docker</t>
+    <t>Cloud</t>
   </si>
   <si>
-    <t>containers</t>
+    <t>AWS</t>
   </si>
   <si>
-    <t>shell</t>
+    <t>AppleUI</t>
   </si>
   <si>
-    <t>Scripting</t>
+    <t>icloud</t>
   </si>
 </sst>
 </file>
@@ -2585,7 +2585,7 @@
       <c r="A4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>